<commit_message>
Finished bar charts and media
Created 6 bar graphs for analysis, new data selection for media sources added
</commit_message>
<xml_diff>
--- a/Excel_File_ElectionSurvey_Keith.xlsx
+++ b/Excel_File_ElectionSurvey_Keith.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keith/Documents/GitHub/Election_Survey_Keith/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103B166D-B091-FF41-9056-C92B877D1472}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44DA3E09-F80A-9940-ADA0-13CA3F706A59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{8DC9A568-6DE7-1A41-B6F2-4720B8FBD104}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{8DC9A568-6DE7-1A41-B6F2-4720B8FBD104}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 Election" sheetId="1" r:id="rId1"/>
     <sheet name="Long Term Elections" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="165">
   <si>
     <t>Variables to include:</t>
   </si>
@@ -439,9 +440,6 @@
     <t>POST: SHOULD THE MINIMUM WAGE BE RAISED, KEPT THE SAME, OR LOWERED</t>
   </si>
   <si>
-    <t xml:space="preserve">VCF0070b </t>
-  </si>
-  <si>
     <t xml:space="preserve">Post interviewer gender </t>
   </si>
   <si>
@@ -515,13 +513,22 @@
   </si>
   <si>
     <t>Variables to include 1948-2016:</t>
+  </si>
+  <si>
+    <t>David Shore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCF0004 </t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,8 +544,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial,Bold"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,8 +563,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -575,20 +593,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -905,656 +953,664 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0ECF1E5-5BD1-5240-A517-2CFD2BF2C284}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="B1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:9">
+      <c r="B1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="2:9">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H40" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E3" s="2" t="s">
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="F46" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="2:3">
+      <c r="B49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="2:3">
+      <c r="B50" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="2:3">
+      <c r="B51" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="2:3">
+      <c r="B52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="2:3">
+      <c r="B53" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="2:3">
+      <c r="B54" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="2:3">
+      <c r="B55" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="2:3">
+      <c r="B56" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="2:3">
+      <c r="B57" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="2:3">
+      <c r="B58" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="2:3">
+      <c r="B59" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="2:3">
+      <c r="B60" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="2:3">
+      <c r="B61" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+    <row r="62" spans="2:3">
+      <c r="B62" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="2:3">
+      <c r="B63" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="2:3">
+      <c r="B64" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="2:3">
+      <c r="B65" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="2:3">
+      <c r="B66" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+    <row r="67" spans="2:3">
+      <c r="B67" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="2:3">
+      <c r="B68" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="2:3">
+      <c r="B69" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="6" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1568,19 +1624,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>